<commit_message>
bổ sung mã quy hoạch vị trí
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/excel-templates/Result_Reg_CSHT.xlsx
+++ b/src/main/webapp/WEB-INF/excel-templates/Result_Reg_CSHT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNPT\RIMS\trunk\code\RIMS\src\main\webapp\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\RIMS\source\RIMS\src\main\webapp\WEB-INF\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FA3D5453-E324-4068-B948-5C69C193CF2F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BIM INFO" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>Thông tin hạ tầng</t>
   </si>
@@ -154,12 +155,15 @@
   </si>
   <si>
     <t>Kết quả</t>
+  </si>
+  <si>
+    <t>Mã quy hoạch vị trí</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -188,7 +192,7 @@
       <b/>
       <sz val="16"/>
       <color indexed="8"/>
-      <name val="Times New Roman"/>
+      <name val="Cambria"/>
       <family val="1"/>
       <charset val="163"/>
       <scheme val="major"/>
@@ -323,42 +327,45 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bad 2 3 2 4" xfId="1"/>
+    <cellStyle name="Bad 2 3 2 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -702,248 +709,252 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AZ4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="57" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" customWidth="1"/>
-    <col min="27" max="27" width="11.42578125" customWidth="1"/>
-    <col min="28" max="28" width="17" customWidth="1"/>
-    <col min="32" max="32" width="10.7109375" customWidth="1"/>
-    <col min="38" max="38" width="13.28515625" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="57" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" customWidth="1"/>
+    <col min="29" max="29" width="17" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" customWidth="1"/>
+    <col min="39" max="39" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:52" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="5"/>
-      <c r="AT1" s="5"/>
-      <c r="AU1" s="5"/>
-      <c r="AV1" s="5"/>
-      <c r="AW1" s="5"/>
-      <c r="AX1" s="5"/>
-      <c r="AY1" s="5"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
     </row>
-    <row r="2" spans="1:51" ht="15" customHeight="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:52" ht="15" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" s="6" t="s">
+      <c r="S2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="W2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA2" s="4" t="s">
+      <c r="X2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AG2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AH2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AN2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AP2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AR2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AS2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AO2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:51" ht="90">
-      <c r="A3" s="13"/>
+    <row r="3" spans="1:52" ht="90">
+      <c r="A3" s="5"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="7"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="9"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -954,120 +965,105 @@
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="7"/>
+      <c r="R3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" s="7"/>
       <c r="AB3" s="7"/>
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7"/>
-      <c r="AF3" s="3" t="s">
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AG3" s="3" t="s">
+      <c r="AH3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AI3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AI3" s="3" t="s">
+      <c r="AJ3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AJ3" s="3" t="s">
+      <c r="AK3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AL3" s="3" t="s">
+      <c r="AM3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AM3" s="3" t="s">
+      <c r="AN3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AN3" s="3" t="s">
+      <c r="AO3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AO3" s="3" t="s">
+      <c r="AP3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AP3" s="3" t="s">
+      <c r="AQ3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AQ3" s="3" t="s">
+      <c r="AR3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AR3" s="3" t="s">
+      <c r="AS3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AS3" s="3" t="s">
+      <c r="AT3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AT3" s="7"/>
       <c r="AU3" s="7"/>
       <c r="AV3" s="7"/>
       <c r="AW3" s="7"/>
       <c r="AX3" s="7"/>
       <c r="AY3" s="7"/>
+      <c r="AZ3" s="7"/>
     </row>
-    <row r="4" spans="1:51" ht="15.75">
-      <c r="F4" s="2"/>
+    <row r="4" spans="1:52" ht="15.75">
+      <c r="G4" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
+  <mergeCells count="33">
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="B1:AZ1"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="AG2:AM2"/>
+    <mergeCell ref="AN2:AT2"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B1:AY1"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="AF2:AL2"/>
-    <mergeCell ref="AM2:AS2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
@@ -1075,6 +1071,23 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>